<commit_message>
Change page orders and significant update on Post-2002 page
</commit_message>
<xml_diff>
--- a/data/exhibition-scrolls.xlsx
+++ b/data/exhibition-scrolls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr updateLinks="always" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efe0c26e679d6e5d/Nettsider/ludvik-a-kjeldsberg.com/The Web of Sites/Academic Research/A Database of Dead Sea Scolls Exhibitions in the 20th and 21st Centuries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hildad/Documents/GitHub/lyingpendatabases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="14_{70F00F1F-2F22-431D-AF12-2590F77F52EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7E2EA48-BD59-4E52-A950-249C37803563}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3634134-9115-EE4E-A7CF-FCA472F0240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29000" yWindow="0" windowWidth="22200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSS Exhibited" sheetId="1" r:id="rId1"/>
@@ -1483,10 +1483,6 @@
     <t>1QapGen</t>
   </si>
   <si>
-    <t xml:space="preserve">Col. I (frag. Pulled from side of scroll)
-</t>
-  </si>
-  <si>
     <r>
       <t>Facsimile of 4Q109 Qoh</t>
     </r>
@@ -1530,6 +1526,9 @@
       </rPr>
       <t>b</t>
     </r>
+  </si>
+  <si>
+    <t>Col. I (frag. Pulled from side of scroll)</t>
   </si>
 </sst>
 </file>
@@ -2316,16 +2315,14 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="DSS Exhibitions"/>
+      <sheetName val="A Database of Dead Sea Scrolls "/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2351,7 +2348,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2652,22 +2649,22 @@
   </sheetPr>
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="53" customWidth="1"/>
-    <col min="5" max="5" width="65.140625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="53" customWidth="1"/>
+    <col min="5" max="5" width="65.1640625" style="50" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>186</v>
       </c>
@@ -2685,7 +2682,7 @@
       </c>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>237</v>
       </c>
@@ -2711,7 +2708,7 @@
       </c>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>237</v>
       </c>
@@ -2737,7 +2734,7 @@
       </c>
       <c r="F3" s="48"/>
     </row>
-    <row r="4" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2758,7 +2755,7 @@
       </c>
       <c r="F4" s="48"/>
     </row>
-    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
@@ -2781,7 +2778,7 @@
       </c>
       <c r="F5" s="48"/>
     </row>
-    <row r="6" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>255</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D6" s="14">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
@@ -2805,7 +2802,7 @@
       </c>
       <c r="F6" s="48"/>
     </row>
-    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2825,7 +2822,7 @@
       </c>
       <c r="F7" s="48"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -2844,7 +2841,7 @@
       </c>
       <c r="F8" s="48"/>
     </row>
-    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2864,7 +2861,7 @@
       </c>
       <c r="F9" s="48"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
@@ -2883,7 +2880,7 @@
       </c>
       <c r="F10" s="48"/>
     </row>
-    <row r="11" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -2903,7 +2900,7 @@
       </c>
       <c r="F11" s="48"/>
     </row>
-    <row r="12" spans="1:6" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2926,7 +2923,7 @@
       </c>
       <c r="F12" s="48"/>
     </row>
-    <row r="13" spans="1:6" ht="351" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="351" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2954,7 +2951,7 @@
       </c>
       <c r="F13" s="48"/>
     </row>
-    <row r="14" spans="1:6" ht="252" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="209" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2983,7 +2980,7 @@
       </c>
       <c r="F14" s="48"/>
     </row>
-    <row r="15" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
@@ -3003,7 +3000,7 @@
       </c>
       <c r="F15" s="48"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3019,7 @@
       </c>
       <c r="F16" s="48"/>
     </row>
-    <row r="17" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -3044,7 +3041,7 @@
       </c>
       <c r="F17" s="48"/>
     </row>
-    <row r="18" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -3065,7 +3062,7 @@
       </c>
       <c r="F18" s="48"/>
     </row>
-    <row r="19" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -3086,12 +3083,12 @@
       </c>
       <c r="F19" s="48"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="43">
@@ -3105,7 +3102,7 @@
       </c>
       <c r="F20" s="48"/>
     </row>
-    <row r="21" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="171" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -3133,7 +3130,7 @@
       </c>
       <c r="F21" s="48"/>
     </row>
-    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>252</v>
       </c>
@@ -3152,7 +3149,7 @@
       </c>
       <c r="F22" s="48"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>157</v>
       </c>
@@ -3171,7 +3168,7 @@
       </c>
       <c r="F23" s="48"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
         <v>157</v>
       </c>
@@ -3190,7 +3187,7 @@
       </c>
       <c r="F24" s="48"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>157</v>
       </c>
@@ -3209,7 +3206,7 @@
       </c>
       <c r="F25" s="48"/>
     </row>
-    <row r="26" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="171" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
         <v>2</v>
       </c>
@@ -3237,7 +3234,7 @@
       </c>
       <c r="F26" s="48"/>
     </row>
-    <row r="27" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -3267,7 +3264,7 @@
       </c>
       <c r="F27" s="48"/>
     </row>
-    <row r="28" spans="1:6" ht="264" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="268" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -3301,7 +3298,7 @@
       </c>
       <c r="F28" s="48"/>
     </row>
-    <row r="29" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="110" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -3327,7 +3324,7 @@
       </c>
       <c r="F29" s="48"/>
     </row>
-    <row r="30" spans="1:6" ht="288" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="227" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -3354,7 +3351,7 @@
       </c>
       <c r="F30" s="48"/>
     </row>
-    <row r="31" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -3380,7 +3377,7 @@
       </c>
       <c r="F31" s="48"/>
     </row>
-    <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="407" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -3420,7 +3417,7 @@
       </c>
       <c r="F32" s="48"/>
     </row>
-    <row r="33" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="220" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>175</v>
       </c>
@@ -3451,7 +3448,7 @@
       </c>
       <c r="F33" s="48"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>157</v>
       </c>
@@ -3470,7 +3467,7 @@
       </c>
       <c r="F34" s="48"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>157</v>
       </c>
@@ -3489,7 +3486,7 @@
       </c>
       <c r="F35" s="48"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>157</v>
       </c>
@@ -3508,7 +3505,7 @@
       </c>
       <c r="F36" s="48"/>
     </row>
-    <row r="37" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>157</v>
       </c>
@@ -3534,7 +3531,7 @@
       </c>
       <c r="F37" s="48"/>
     </row>
-    <row r="38" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="81" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>157</v>
       </c>
@@ -3557,7 +3554,7 @@
       </c>
       <c r="F38" s="48"/>
     </row>
-    <row r="39" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>157</v>
       </c>
@@ -3583,7 +3580,7 @@
       </c>
       <c r="F39" s="48"/>
     </row>
-    <row r="40" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>157</v>
       </c>
@@ -3610,7 +3607,7 @@
       </c>
       <c r="F40" s="48"/>
     </row>
-    <row r="41" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>157</v>
       </c>
@@ -3631,7 +3628,7 @@
       </c>
       <c r="F41" s="48"/>
     </row>
-    <row r="42" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>157</v>
       </c>
@@ -3652,7 +3649,7 @@
       </c>
       <c r="F42" s="48"/>
     </row>
-    <row r="43" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>157</v>
       </c>
@@ -3673,7 +3670,7 @@
       </c>
       <c r="F43" s="48"/>
     </row>
-    <row r="44" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>157</v>
       </c>
@@ -3694,7 +3691,7 @@
       </c>
       <c r="F44" s="48"/>
     </row>
-    <row r="45" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>157</v>
       </c>
@@ -3720,7 +3717,7 @@
       </c>
       <c r="F45" s="48"/>
     </row>
-    <row r="46" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="81" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>157</v>
       </c>
@@ -3743,7 +3740,7 @@
       </c>
       <c r="F46" s="48"/>
     </row>
-    <row r="47" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>157</v>
       </c>
@@ -3769,7 +3766,7 @@
       </c>
       <c r="F47" s="48"/>
     </row>
-    <row r="48" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="220" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>157</v>
       </c>
@@ -3800,7 +3797,7 @@
       </c>
       <c r="F48" s="48"/>
     </row>
-    <row r="49" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>157</v>
       </c>
@@ -3827,7 +3824,7 @@
       </c>
       <c r="F49" s="48"/>
     </row>
-    <row r="50" spans="1:6" ht="99" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>157</v>
       </c>
@@ -3851,7 +3848,7 @@
       </c>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:6" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>157</v>
       </c>
@@ -3876,7 +3873,7 @@
       </c>
       <c r="F51" s="48"/>
     </row>
-    <row r="52" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>157</v>
       </c>
@@ -3901,7 +3898,7 @@
       </c>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>157</v>
       </c>
@@ -3922,7 +3919,7 @@
       </c>
       <c r="F53" s="48"/>
     </row>
-    <row r="54" spans="1:6" ht="255.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="268" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>157</v>
       </c>
@@ -3956,7 +3953,7 @@
       </c>
       <c r="F54" s="48"/>
     </row>
-    <row r="55" spans="1:6" ht="239.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="252" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>157</v>
       </c>
@@ -3991,7 +3988,7 @@
       </c>
       <c r="F55" s="48"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>157</v>
       </c>
@@ -4010,7 +4007,7 @@
       </c>
       <c r="F56" s="48"/>
     </row>
-    <row r="57" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>157</v>
       </c>
@@ -4035,7 +4032,7 @@
       </c>
       <c r="F57" s="48"/>
     </row>
-    <row r="58" spans="1:6" ht="231" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="236" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>157</v>
       </c>
@@ -4067,7 +4064,7 @@
       </c>
       <c r="F58" s="48"/>
     </row>
-    <row r="59" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>157</v>
       </c>
@@ -4089,7 +4086,7 @@
       </c>
       <c r="F59" s="48"/>
     </row>
-    <row r="60" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="188" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>157</v>
       </c>
@@ -4118,7 +4115,7 @@
       </c>
       <c r="F60" s="48"/>
     </row>
-    <row r="61" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>157</v>
       </c>
@@ -4143,7 +4140,7 @@
       </c>
       <c r="F61" s="48"/>
     </row>
-    <row r="62" spans="1:6" ht="99" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>157</v>
       </c>
@@ -4167,7 +4164,7 @@
       </c>
       <c r="F62" s="48"/>
     </row>
-    <row r="63" spans="1:6" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>157</v>
       </c>
@@ -4192,7 +4189,7 @@
       </c>
       <c r="F63" s="48"/>
     </row>
-    <row r="64" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>157</v>
       </c>
@@ -4217,7 +4214,7 @@
       </c>
       <c r="F64" s="48"/>
     </row>
-    <row r="65" spans="1:6" ht="99" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>157</v>
       </c>
@@ -4241,7 +4238,7 @@
       </c>
       <c r="F65" s="48"/>
     </row>
-    <row r="66" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>157</v>
       </c>
@@ -4263,7 +4260,7 @@
       </c>
       <c r="F66" s="48"/>
     </row>
-    <row r="67" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="188" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>157</v>
       </c>
@@ -4292,7 +4289,7 @@
       </c>
       <c r="F67" s="48"/>
     </row>
-    <row r="68" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>157</v>
       </c>
@@ -4312,7 +4309,7 @@
       </c>
       <c r="F68" s="48"/>
     </row>
-    <row r="69" spans="1:6" ht="99" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>157</v>
       </c>
@@ -4336,7 +4333,7 @@
       </c>
       <c r="F69" s="48"/>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>157</v>
       </c>
@@ -4355,7 +4352,7 @@
       </c>
       <c r="F70" s="48"/>
     </row>
-    <row r="71" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>157</v>
       </c>
@@ -4375,7 +4372,7 @@
       </c>
       <c r="F71" s="48"/>
     </row>
-    <row r="72" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>157</v>
       </c>
@@ -4395,7 +4392,7 @@
       </c>
       <c r="F72" s="48"/>
     </row>
-    <row r="73" spans="1:6" ht="189.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>157</v>
       </c>
@@ -4425,7 +4422,7 @@
       </c>
       <c r="F73" s="48"/>
     </row>
-    <row r="74" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>157</v>
       </c>
@@ -4450,7 +4447,7 @@
       </c>
       <c r="F74" s="48"/>
     </row>
-    <row r="75" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>157</v>
       </c>
@@ -4471,7 +4468,7 @@
       </c>
       <c r="F75" s="48"/>
     </row>
-    <row r="76" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>157</v>
       </c>
@@ -4497,7 +4494,7 @@
       </c>
       <c r="F76" s="48"/>
     </row>
-    <row r="77" spans="1:6" ht="99" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
@@ -4521,7 +4518,7 @@
       </c>
       <c r="F77" s="48"/>
     </row>
-    <row r="78" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>157</v>
       </c>
@@ -4546,7 +4543,7 @@
       </c>
       <c r="F78" s="48"/>
     </row>
-    <row r="79" spans="1:6" ht="255.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="268" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>157</v>
       </c>
@@ -4580,7 +4577,7 @@
       </c>
       <c r="F79" s="48"/>
     </row>
-    <row r="80" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
@@ -4600,7 +4597,7 @@
       </c>
       <c r="F80" s="48"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>157</v>
       </c>
@@ -4619,7 +4616,7 @@
       </c>
       <c r="F81" s="48"/>
     </row>
-    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>157</v>
       </c>
@@ -4638,7 +4635,7 @@
       </c>
       <c r="F82" s="49"/>
     </row>
-    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>157</v>
       </c>
@@ -4657,12 +4654,12 @@
       </c>
       <c r="F83" s="49"/>
     </row>
-    <row r="84" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="81" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>157</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="13">
@@ -4680,7 +4677,7 @@
       </c>
       <c r="F84" s="49"/>
     </row>
-    <row r="85" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>157</v>
       </c>
@@ -4707,7 +4704,7 @@
       </c>
       <c r="F85" s="48"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>171</v>
       </c>
@@ -4726,12 +4723,12 @@
       </c>
       <c r="F86" s="48"/>
     </row>
-    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="14">
@@ -4745,12 +4742,12 @@
       </c>
       <c r="F87" s="48"/>
     </row>
-    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="14">
@@ -4764,12 +4761,12 @@
       </c>
       <c r="F88" s="48"/>
     </row>
-    <row r="89" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="14">
@@ -4783,7 +4780,7 @@
       </c>
       <c r="F89" s="48"/>
     </row>
-    <row r="90" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -4805,7 +4802,7 @@
       </c>
       <c r="F90" s="48"/>
     </row>
-    <row r="91" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -4827,7 +4824,7 @@
       </c>
       <c r="F91" s="48"/>
     </row>
-    <row r="92" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
@@ -4848,7 +4845,7 @@
       </c>
       <c r="F92" s="48"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
@@ -4867,7 +4864,7 @@
       </c>
       <c r="F93" s="48"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>12</v>
       </c>
@@ -4886,7 +4883,7 @@
       </c>
       <c r="F94" s="48"/>
     </row>
-    <row r="95" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
@@ -4909,7 +4906,7 @@
       </c>
       <c r="F95" s="48"/>
     </row>
-    <row r="96" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>12</v>
       </c>
@@ -4932,7 +4929,7 @@
       </c>
       <c r="F96" s="48"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>181</v>
       </c>
@@ -4951,7 +4948,7 @@
       </c>
       <c r="F97" s="48"/>
     </row>
-    <row r="98" spans="1:6" ht="74.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="81" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>181</v>
       </c>
@@ -4974,7 +4971,7 @@
       </c>
       <c r="F98" s="48"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>181</v>
       </c>
@@ -4993,7 +4990,7 @@
       </c>
       <c r="F99" s="48"/>
     </row>
-    <row r="100" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>181</v>
       </c>
@@ -5012,7 +5009,7 @@
       </c>
       <c r="F100" s="48"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>19</v>
       </c>
@@ -5033,7 +5030,7 @@
       </c>
       <c r="F101" s="48"/>
     </row>
-    <row r="102" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>19</v>
       </c>
@@ -5061,7 +5058,7 @@
       </c>
       <c r="F102" s="48"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>19</v>
       </c>
@@ -5080,7 +5077,7 @@
       </c>
       <c r="F103" s="48"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>19</v>
       </c>
@@ -5099,7 +5096,7 @@
       </c>
       <c r="F104" s="48"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>19</v>
       </c>
@@ -5120,7 +5117,7 @@
       </c>
       <c r="F105" s="48"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>19</v>
       </c>
@@ -5141,7 +5138,7 @@
       </c>
       <c r="F106" s="48"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>19</v>
       </c>
@@ -5160,7 +5157,7 @@
       </c>
       <c r="F107" s="48"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>19</v>
       </c>
@@ -5181,7 +5178,7 @@
       </c>
       <c r="F108" s="48"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>19</v>
       </c>
@@ -5202,7 +5199,7 @@
       </c>
       <c r="F109" s="48"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>19</v>
       </c>
@@ -5223,7 +5220,7 @@
       </c>
       <c r="F110" s="48"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>19</v>
       </c>
@@ -5244,7 +5241,7 @@
       </c>
       <c r="F111" s="48"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
@@ -5265,7 +5262,7 @@
       </c>
       <c r="F112" s="48"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -5286,7 +5283,7 @@
       </c>
       <c r="F113" s="48"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>19</v>
       </c>
@@ -5307,7 +5304,7 @@
       </c>
       <c r="F114" s="48"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>19</v>
       </c>
@@ -5328,7 +5325,7 @@
       </c>
       <c r="F115" s="48"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>19</v>
       </c>
@@ -5349,7 +5346,7 @@
       </c>
       <c r="F116" s="48"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>19</v>
       </c>
@@ -5370,7 +5367,7 @@
       </c>
       <c r="F117" s="48"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>19</v>
       </c>
@@ -5391,7 +5388,7 @@
       </c>
       <c r="F118" s="48"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>19</v>
       </c>
@@ -5410,7 +5407,7 @@
       </c>
       <c r="F119" s="48"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>19</v>
       </c>
@@ -5431,7 +5428,7 @@
       </c>
       <c r="F120" s="48"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>19</v>
       </c>
@@ -5452,7 +5449,7 @@
       </c>
       <c r="F121" s="48"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>19</v>
       </c>
@@ -5473,7 +5470,7 @@
       </c>
       <c r="F122" s="48"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>19</v>
       </c>
@@ -5494,7 +5491,7 @@
       </c>
       <c r="F123" s="48"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>19</v>
       </c>
@@ -5515,7 +5512,7 @@
       </c>
       <c r="F124" s="48"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>19</v>
       </c>
@@ -5536,7 +5533,7 @@
       </c>
       <c r="F125" s="48"/>
     </row>
-    <row r="126" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>19</v>
       </c>
@@ -5556,7 +5553,7 @@
       </c>
       <c r="F126" s="48"/>
     </row>
-    <row r="127" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>19</v>
       </c>
@@ -5578,7 +5575,7 @@
       </c>
       <c r="F127" s="48"/>
     </row>
-    <row r="128" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>19</v>
       </c>
@@ -5600,7 +5597,7 @@
       </c>
       <c r="F128" s="48"/>
     </row>
-    <row r="129" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>19</v>
       </c>
@@ -5621,7 +5618,7 @@
       </c>
       <c r="F129" s="48"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>19</v>
       </c>
@@ -5642,7 +5639,7 @@
       </c>
       <c r="F130" s="48"/>
     </row>
-    <row r="131" spans="1:6" ht="74.25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="81" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>19</v>
       </c>
@@ -5667,7 +5664,7 @@
       </c>
       <c r="F131" s="48"/>
     </row>
-    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>19</v>
       </c>
@@ -5688,7 +5685,7 @@
       </c>
       <c r="F132" s="48"/>
     </row>
-    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>19</v>
       </c>
@@ -5709,7 +5706,7 @@
       </c>
       <c r="F133" s="48"/>
     </row>
-    <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>19</v>
       </c>
@@ -5730,7 +5727,7 @@
       </c>
       <c r="F134" s="48"/>
     </row>
-    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>19</v>
       </c>
@@ -5751,7 +5748,7 @@
       </c>
       <c r="F135" s="48"/>
     </row>
-    <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>19</v>
       </c>
@@ -5772,7 +5769,7 @@
       </c>
       <c r="F136" s="48"/>
     </row>
-    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>19</v>
       </c>
@@ -5793,7 +5790,7 @@
       </c>
       <c r="F137" s="48"/>
     </row>
-    <row r="138" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>19</v>
       </c>
@@ -5814,7 +5811,7 @@
       </c>
       <c r="F138" s="48"/>
     </row>
-    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>19</v>
       </c>
@@ -5833,7 +5830,7 @@
       </c>
       <c r="F139" s="48"/>
     </row>
-    <row r="140" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>19</v>
       </c>
@@ -5854,7 +5851,7 @@
       </c>
       <c r="F140" s="48"/>
     </row>
-    <row r="141" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>19</v>
       </c>
@@ -5876,7 +5873,7 @@
       </c>
       <c r="F141" s="48"/>
     </row>
-    <row r="142" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>19</v>
       </c>
@@ -5902,7 +5899,7 @@
       </c>
       <c r="F142" s="48"/>
     </row>
-    <row r="143" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>19</v>
       </c>
@@ -5926,7 +5923,7 @@
       </c>
       <c r="F143" s="48"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>19</v>
       </c>
@@ -5947,7 +5944,7 @@
       </c>
       <c r="F144" s="48"/>
     </row>
-    <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>19</v>
       </c>
@@ -5968,7 +5965,7 @@
       </c>
       <c r="F145" s="48"/>
     </row>
-    <row r="146" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>19</v>
       </c>
@@ -5991,7 +5988,7 @@
       </c>
       <c r="F146" s="48"/>
     </row>
-    <row r="147" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>19</v>
       </c>
@@ -6013,7 +6010,7 @@
       </c>
       <c r="F147" s="48"/>
     </row>
-    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>19</v>
       </c>
@@ -6034,7 +6031,7 @@
       </c>
       <c r="F148" s="48"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>19</v>
       </c>
@@ -6055,7 +6052,7 @@
       </c>
       <c r="F149" s="48"/>
     </row>
-    <row r="150" spans="1:6" ht="305.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>19</v>
       </c>
@@ -6079,7 +6076,7 @@
       </c>
       <c r="F150" s="48"/>
     </row>
-    <row r="151" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>19</v>
       </c>
@@ -6102,7 +6099,7 @@
       </c>
       <c r="F151" s="48"/>
     </row>
-    <row r="152" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>19</v>
       </c>
@@ -6124,7 +6121,7 @@
       </c>
       <c r="F152" s="48"/>
     </row>
-    <row r="153" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>19</v>
       </c>
@@ -6147,7 +6144,7 @@
       </c>
       <c r="F153" s="48"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>19</v>
       </c>
@@ -6168,7 +6165,7 @@
       </c>
       <c r="F154" s="48"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>19</v>
       </c>
@@ -6189,7 +6186,7 @@
       </c>
       <c r="F155" s="48"/>
     </row>
-    <row r="156" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>19</v>
       </c>
@@ -6208,7 +6205,7 @@
       </c>
       <c r="F156" s="48"/>
     </row>
-    <row r="157" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>19</v>
       </c>
@@ -6227,7 +6224,7 @@
       </c>
       <c r="F157" s="48"/>
     </row>
-    <row r="158" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>19</v>
       </c>
@@ -6255,7 +6252,7 @@
       </c>
       <c r="F158" s="48"/>
     </row>
-    <row r="159" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>19</v>
       </c>
@@ -6276,7 +6273,7 @@
       </c>
       <c r="F159" s="48"/>
     </row>
-    <row r="160" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>19</v>
       </c>
@@ -6297,7 +6294,7 @@
       </c>
       <c r="F160" s="48"/>
     </row>
-    <row r="161" spans="1:6" ht="239.25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="252" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>19</v>
       </c>
@@ -6332,7 +6329,7 @@
       </c>
       <c r="F161" s="48"/>
     </row>
-    <row r="162" spans="1:6" ht="247.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="252" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>19</v>
       </c>
@@ -6367,7 +6364,7 @@
       </c>
       <c r="F162" s="48"/>
     </row>
-    <row r="163" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>19</v>
       </c>
@@ -6395,7 +6392,7 @@
       </c>
       <c r="F163" s="48"/>
     </row>
-    <row r="164" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>19</v>
       </c>
@@ -6416,7 +6413,7 @@
       </c>
       <c r="F164" s="48"/>
     </row>
-    <row r="165" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>19</v>
       </c>
@@ -6437,7 +6434,7 @@
       </c>
       <c r="F165" s="48"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>19</v>
       </c>
@@ -6458,7 +6455,7 @@
       </c>
       <c r="F166" s="48"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>19</v>
       </c>
@@ -6479,7 +6476,7 @@
       </c>
       <c r="F167" s="48"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>19</v>
       </c>
@@ -6500,7 +6497,7 @@
       </c>
       <c r="F168" s="48"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>19</v>
       </c>
@@ -6521,7 +6518,7 @@
       </c>
       <c r="F169" s="48"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>19</v>
       </c>
@@ -6542,7 +6539,7 @@
       </c>
       <c r="F170" s="48"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>19</v>
       </c>
@@ -6563,7 +6560,7 @@
       </c>
       <c r="F171" s="48"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>19</v>
       </c>
@@ -6584,7 +6581,7 @@
       </c>
       <c r="F172" s="48"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>19</v>
       </c>
@@ -6605,7 +6602,7 @@
       </c>
       <c r="F173" s="48"/>
     </row>
-    <row r="174" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>19</v>
       </c>
@@ -6626,7 +6623,7 @@
       </c>
       <c r="F174" s="48"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="25" t="s">
         <v>19</v>
       </c>
@@ -6645,7 +6642,7 @@
       </c>
       <c r="F175" s="48"/>
     </row>
-    <row r="176" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="54" x14ac:dyDescent="0.2">
       <c r="A176" s="26" t="s">
         <v>19</v>
       </c>
@@ -6668,7 +6665,7 @@
       </c>
       <c r="F176" s="48"/>
     </row>
-    <row r="177" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A177" s="26" t="s">
         <v>43</v>
       </c>
@@ -6694,7 +6691,7 @@
       </c>
       <c r="F177" s="48"/>
     </row>
-    <row r="178" spans="1:6" ht="256.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="256.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="26" t="s">
         <v>173</v>
       </c>
@@ -6717,7 +6714,7 @@
       </c>
       <c r="F178" s="48"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="24"/>
       <c r="B179" s="22"/>
       <c r="C179" s="3"/>
@@ -6732,7 +6729,7 @@
       </c>
       <c r="F179" s="49"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="24"/>
       <c r="B180" s="22"/>
       <c r="C180" s="3"/>
@@ -6747,7 +6744,7 @@
       </c>
       <c r="F180" s="49"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="24"/>
       <c r="B181" s="22"/>
       <c r="C181" s="3"/>
@@ -6762,7 +6759,7 @@
       </c>
       <c r="F181" s="49"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="24"/>
       <c r="B182" s="22"/>
       <c r="C182" s="3"/>
@@ -6777,7 +6774,7 @@
       </c>
       <c r="F182" s="49"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="24"/>
       <c r="B183" s="22"/>
       <c r="C183" s="3"/>
@@ -6792,7 +6789,7 @@
       </c>
       <c r="F183" s="49"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="24"/>
       <c r="B184" s="22"/>
       <c r="C184" s="3"/>
@@ -6807,7 +6804,7 @@
       </c>
       <c r="F184" s="49"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="23"/>
       <c r="B185" s="21"/>
       <c r="C185" s="10"/>

</xml_diff>